<commit_message>
gui/cli io bugfixes; Pillow 10+ font.getsize() fix; --titleblock now applicable to --adproject.
</commit_message>
<xml_diff>
--- a/example/AD project/project outputs/Bill of Materials/BCAD.123456.001 СК [config 2].xlsx
+++ b/example/AD project/project outputs/Bill of Materials/BCAD.123456.001 СК [config 2].xlsx
@@ -153,7 +153,7 @@
     <t>керам., чип 0603, X7R, 0.068мкФ ±10%, 50В</t>
   </si>
   <si>
-    <t>C2, C9, C10, C11, C14, C15, C17, C18, C19D, C19E, C19F, C19G, C19B, C19A, C19C, C20A, C20B, C20C, C21A, C22B, C22C, C22G, C22A, C22F, C22D, C22E, C23B, C23A, C23G, C23C, C23F, C23E, C23D, C24E, C24F, C24G, C24A, C24B, C24C, C24D</t>
+    <t>C2, C9, C10, C11, C14, C15, C17, C18, C19G, C19F, C19E, C19A, C19B, C19D, C19C, C20A, C20B, C20C, C21A, C22B, C22D, C22C, C22F, C22E, C22G, C22A, C23A, C23B, C23C, C23D, C23E, C23F, C23G, C24C, C24E, C24D, C24A, C24B, C24G, C24F</t>
   </si>
   <si>
     <t>CC0603KRX7R9BB104</t>
@@ -162,7 +162,7 @@
     <t>керам., чип 0603, X7R, 0.1мкФ ±10%, 50В</t>
   </si>
   <si>
-    <t>C20F, C20D, C20E, C20G</t>
+    <t>C20G, C20F, C20E, C20D</t>
   </si>
   <si>
     <t>CC0603KRX7R9BB224</t>

</xml_diff>